<commit_message>
fixed figure numbering in code and source data for final submission
</commit_message>
<xml_diff>
--- a/figures/source_data/source_Fig.3c.xlsx
+++ b/figures/source_data/source_Fig.3c.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.45 (µg/ml)</t>
+          <t>0.225 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.45 (µg/ml)</t>
+          <t>0.225 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.45 (µg/ml)</t>
+          <t>0.225 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.45 (µg/ml)</t>
+          <t>0.225 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.9 (µg/ml)</t>
+          <t>0.45 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.9 (µg/ml)</t>
+          <t>0.45 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.9 (µg/ml)</t>
+          <t>0.45 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.9 (µg/ml)</t>
+          <t>0.45 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.8 (µg/ml)</t>
+          <t>0.9 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.8 (µg/ml)</t>
+          <t>0.9 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.8 (µg/ml)</t>
+          <t>0.9 (µg/ml)</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.8 (µg/ml)</t>
+          <t>0.9 (µg/ml)</t>
         </is>
       </c>
     </row>

</xml_diff>